<commit_message>
updated timing after running benchmarks again against other languages
</commit_message>
<xml_diff>
--- a/objeck-lang/wip/timming/times.xlsx
+++ b/objeck-lang/wip/timming/times.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="2940" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="960" yWindow="2940" windowWidth="20740" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -38,6 +38,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10"/>
@@ -96,7 +102,24 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Prime Numbers: 1-1,000,000</a:t>
+              <a:t>Prime Numbers: 1-1,000,000 </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>(OSX 10.6 - 2.93</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t> Intel Core 2 Duo</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -127,10 +150,10 @@
                   <c:v>Objeck (Interpreted)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Objeck (JIT)</c:v>
+                  <c:v>Java 1.6 (JIT)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Java 1.6 (JIT)</c:v>
+                  <c:v>Objeck (JIT)</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>g++ 4.2 (-02)</c:v>
@@ -145,39 +168,39 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>18.88205</c:v>
+                  <c:v>21.064175</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.93206224999999998</c:v>
+                  <c:v>0.90075</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.90074999999999994</c:v>
+                  <c:v>0.8684915</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.38547824999999997</c:v>
+                  <c:v>0.38547825</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="75283072"/>
-        <c:axId val="75363840"/>
+        <c:axId val="541783864"/>
+        <c:axId val="541787192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75283072"/>
+        <c:axId val="541783864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75363840"/>
+        <c:crossAx val="541787192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75363840"/>
+        <c:axId val="541787192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -185,14 +208,23 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75283072"/>
+        <c:crossAx val="541783864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.832484620369466"/>
+          <c:y val="0.491330259193288"/>
+          <c:w val="0.141272803131852"/>
+          <c:h val="0.130624427760483"/>
+        </c:manualLayout>
+      </c:layout>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -210,14 +242,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>101601</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -558,19 +590,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -578,10 +609,10 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -589,13 +620,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>18.883900000000001</v>
+        <v>21.063600000000001</v>
       </c>
       <c r="B2">
-        <v>0.93162100000000003</v>
+        <v>0.877</v>
       </c>
       <c r="C2">
-        <v>0.877</v>
+        <v>0.86802199999999996</v>
       </c>
       <c r="D2">
         <v>0.38568599999999997</v>
@@ -603,13 +634,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>18.8809</v>
+        <v>21.0642</v>
       </c>
       <c r="B3">
-        <v>0.92942000000000002</v>
+        <v>0.88300000000000001</v>
       </c>
       <c r="C3">
-        <v>0.88300000000000001</v>
+        <v>0.86253899999999994</v>
       </c>
       <c r="D3">
         <v>0.38621100000000003</v>
@@ -617,13 +648,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>18.881499999999999</v>
+        <v>21.0655</v>
       </c>
       <c r="B4">
-        <v>0.93776000000000004</v>
+        <v>0.93100000000000005</v>
       </c>
       <c r="C4">
-        <v>0.93100000000000005</v>
+        <v>0.87425799999999998</v>
       </c>
       <c r="D4">
         <v>0.38455899999999998</v>
@@ -631,13 +662,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>18.881900000000002</v>
+        <v>21.063400000000001</v>
       </c>
       <c r="B5">
-        <v>0.92944800000000005</v>
+        <v>0.91200000000000003</v>
       </c>
       <c r="C5">
-        <v>0.91200000000000003</v>
+        <v>0.869147</v>
       </c>
       <c r="D5">
         <v>0.38545699999999999</v>
@@ -646,30 +677,25 @@
     <row r="6" spans="1:4">
       <c r="A6">
         <f>AVERAGE(A2:A5)</f>
-        <v>18.88205</v>
+        <v>21.064174999999999</v>
       </c>
       <c r="B6">
         <f>AVERAGE(B2:B5)</f>
-        <v>0.93206224999999998</v>
+        <v>0.90074999999999994</v>
       </c>
       <c r="C6">
         <f>AVERAGE(C2:C5)</f>
-        <v>0.90074999999999994</v>
+        <v>0.86849149999999997</v>
       </c>
       <c r="D6">
         <f>AVERAGE(D2:D5)</f>
         <v>0.38547824999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="C14">
-        <f>1-D6/A6</f>
-        <v>0.97958493648729883</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
updating timings based upon method inlining
</commit_message>
<xml_diff>
--- a/objeck-lang/wip/timming/times.xlsx
+++ b/objeck-lang/wip/timming/times.xlsx
@@ -168,7 +168,7 @@
                   <c:v>0.90075</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8684915</c:v>
+                  <c:v>0.478394</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.38547825</c:v>
@@ -177,24 +177,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="546246792"/>
-        <c:axId val="546238712"/>
+        <c:axId val="565214840"/>
+        <c:axId val="565203480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="546246792"/>
+        <c:axId val="565214840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="546238712"/>
+        <c:crossAx val="565203480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="546238712"/>
+        <c:axId val="565203480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -202,7 +202,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="546246792"/>
+        <c:crossAx val="565214840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -588,7 +588,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
@@ -620,7 +620,7 @@
         <v>0.877</v>
       </c>
       <c r="C2">
-        <v>0.86802199999999996</v>
+        <v>0.47585300000000003</v>
       </c>
       <c r="D2">
         <v>0.38568599999999997</v>
@@ -634,7 +634,7 @@
         <v>0.88300000000000001</v>
       </c>
       <c r="C3">
-        <v>0.86253899999999994</v>
+        <v>0.48208499999999999</v>
       </c>
       <c r="D3">
         <v>0.38621100000000003</v>
@@ -648,7 +648,7 @@
         <v>0.93100000000000005</v>
       </c>
       <c r="C4">
-        <v>0.87425799999999998</v>
+        <v>0.47908600000000001</v>
       </c>
       <c r="D4">
         <v>0.38455899999999998</v>
@@ -662,7 +662,7 @@
         <v>0.91200000000000003</v>
       </c>
       <c r="C5">
-        <v>0.869147</v>
+        <v>0.47655199999999998</v>
       </c>
       <c r="D5">
         <v>0.38545699999999999</v>
@@ -679,7 +679,7 @@
       </c>
       <c r="C6">
         <f>AVERAGE(C2:C5)</f>
-        <v>0.86849149999999997</v>
+        <v>0.47839399999999999</v>
       </c>
       <c r="D6">
         <f>AVERAGE(D2:D5)</f>
@@ -689,10 +689,11 @@
     <row r="8" spans="1:4">
       <c r="A8">
         <f>ABS(C6/A6-1)</f>
-        <v>0.947658611478154</v>
+        <v>0.97116862258235115</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>